<commit_message>
Update and test experiment
</commit_message>
<xml_diff>
--- a/stim_table_test.xlsx
+++ b/stim_table_test.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://penno365-my.sharepoint.com/personal/tuna28ng_upenn_edu/Documents/Documents/GitHub/AO_human_v_robot_main/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\anhtn\OneDrive - PennO365\Documents\GitHub\AO_human_v_robot_main\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="81" documentId="8_{06C59399-4CE5-44E9-8912-D6CF8B75EA6A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{5F8C0682-7059-4FD4-8B5E-0672CFE9C9A3}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B526D20A-D75D-42F5-AA0E-B0EBE116D7C0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="7485" yWindow="2595" windowWidth="19125" windowHeight="14655" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1560" yWindow="1560" windowWidth="21600" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -296,28 +296,7 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="2">
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-  </dxfs>
+  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -328,10 +307,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -600,7 +575,7 @@
   <dimension ref="A1:H27"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E15" sqref="E15"/>
+      <selection activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -616,7 +591,7 @@
     <col min="9" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>54</v>
       </c>
@@ -642,7 +617,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="2" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>0</v>
       </c>
@@ -668,7 +643,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="3" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>0</v>
       </c>
@@ -676,7 +651,7 @@
         <v>55</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>53</v>
+        <v>43</v>
       </c>
       <c r="G3" s="1">
         <v>100</v>
@@ -685,7 +660,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="4" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>0</v>
       </c>
@@ -711,7 +686,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="5" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>1</v>
       </c>
@@ -737,7 +712,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="6" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <v>1</v>
       </c>
@@ -745,7 +720,7 @@
         <v>55</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>53</v>
+        <v>43</v>
       </c>
       <c r="G6" s="1">
         <v>100</v>
@@ -754,7 +729,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="7" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
         <v>1</v>
       </c>
@@ -780,7 +755,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="8" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
         <v>1</v>
       </c>
@@ -806,7 +781,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="9" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
         <v>2</v>
       </c>
@@ -832,7 +807,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="10" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
         <v>2</v>
       </c>
@@ -858,7 +833,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="11" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
         <v>3</v>
       </c>
@@ -884,7 +859,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="12" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
         <v>3</v>
       </c>
@@ -910,7 +885,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="13" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
         <v>4</v>
       </c>
@@ -936,7 +911,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="14" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" s="1">
         <v>4</v>
       </c>
@@ -962,7 +937,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="15" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" s="1">
         <v>4</v>
       </c>
@@ -988,7 +963,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="16" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16" s="1">
         <v>5</v>
       </c>
@@ -1014,7 +989,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="17" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17" s="1">
         <v>5</v>
       </c>
@@ -1040,7 +1015,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="18" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A18" s="1">
         <v>6</v>
       </c>
@@ -1066,7 +1041,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="19" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A19" s="1">
         <v>6</v>
       </c>
@@ -1092,7 +1067,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="20" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A20" s="1">
         <v>6</v>
       </c>
@@ -1118,7 +1093,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="21" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A21" s="1">
         <v>6</v>
       </c>
@@ -1144,7 +1119,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="22" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A22" s="1">
         <v>7</v>
       </c>
@@ -1170,7 +1145,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="23" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A23" s="1">
         <v>7</v>
       </c>
@@ -1196,7 +1171,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="24" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A24" s="1">
         <v>8</v>
       </c>
@@ -1222,7 +1197,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="25" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A25" s="1">
         <v>8</v>
       </c>
@@ -1248,7 +1223,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="26" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A26" s="1">
         <v>9</v>
       </c>
@@ -1274,7 +1249,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="27" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A27" s="1">
         <v>9</v>
       </c>

</xml_diff>

<commit_message>
add emotiv components to experiment
</commit_message>
<xml_diff>
--- a/stim_table_test.xlsx
+++ b/stim_table_test.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\anhtn\OneDrive - PennO365\Documents\GitHub\AO_human_v_robot_main\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://penno365-my.sharepoint.com/personal/tuna28ng_upenn_edu/Documents/Documents/GitHub/AO_human_v_robot_main/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B526D20A-D75D-42F5-AA0E-B0EBE116D7C0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="3" documentId="13_ncr:1_{B526D20A-D75D-42F5-AA0E-B0EBE116D7C0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{CE2872B6-8DFD-42E8-8352-360B46FA1FEE}"/>
   <bookViews>
-    <workbookView xWindow="1560" yWindow="1560" windowWidth="21600" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-31935" yWindow="1170" windowWidth="21600" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="132" uniqueCount="70">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="132" uniqueCount="67">
   <si>
     <t>stimDir</t>
   </si>
@@ -227,25 +227,16 @@
     <t>Landscape 1</t>
   </si>
   <si>
-    <t>./stimuli/control_0.mp4</t>
-  </si>
-  <si>
     <t>control_1</t>
   </si>
   <si>
     <t>Landscape 2</t>
   </si>
   <si>
-    <t>./stimuli/control_1.mp4</t>
-  </si>
-  <si>
     <t>control_2</t>
   </si>
   <si>
     <t>Landscape 3</t>
-  </si>
-  <si>
-    <t>./stimuli/control_2.mp4</t>
   </si>
 </sst>
 </file>
@@ -574,8 +565,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H27"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F7" sqref="F7"/>
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="F14" sqref="F14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1188,7 +1179,7 @@
         <v>62</v>
       </c>
       <c r="F24" s="1" t="s">
-        <v>63</v>
+        <v>52</v>
       </c>
       <c r="G24" s="1">
         <v>50</v>
@@ -1205,16 +1196,16 @@
         <v>60</v>
       </c>
       <c r="C25" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="D25" s="1">
+        <v>1</v>
+      </c>
+      <c r="E25" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="D25" s="1">
-        <v>1</v>
-      </c>
-      <c r="E25" s="1" t="s">
-        <v>65</v>
-      </c>
       <c r="F25" s="1" t="s">
-        <v>66</v>
+        <v>52</v>
       </c>
       <c r="G25" s="1">
         <v>51</v>
@@ -1231,16 +1222,16 @@
         <v>60</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="D26" s="1">
         <v>2</v>
       </c>
       <c r="E26" s="1" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="F26" s="1" t="s">
-        <v>69</v>
+        <v>52</v>
       </c>
       <c r="G26" s="1">
         <v>52</v>

</xml_diff>